<commit_message>
Added necessary files for prototype 1, and wrote all function headers.
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/bronson_billing_utas_edu_au/Documents/2025 - S1/KIT205/KIT205_575952/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{A0285DF0-F68A-42CE-9430-462A5BA0CC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63109568-89D2-4A8F-9161-92C5B8430F3E}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{A0285DF0-F68A-42CE-9430-462A5BA0CC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFECC979-F2DE-46D5-83C0-BF56C61D0C76}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -69,10 +69,6 @@
 1/08/2024</t>
   </si>
   <si>
-    <t>5/8/2024
-8/8/2024</t>
-  </si>
-  <si>
     <t>linked_list_test - tests insertion in empty and large linked lists; deletion from the front, middle, and rear</t>
   </si>
   <si>
@@ -85,28 +81,6 @@
     <t>Functions implented/updated</t>
   </si>
   <si>
-    <t>BST implementation for books.  BST nodes contain the book title as well as linke list of strings for borrowers.</t>
-  </si>
-  <si>
-    <t>new_book (empty list of borrowers)
-new_bst
-insert_bst (sorted by book title)
-delete_bst
-destroy_bst
-find_bst
-print_bst(initial implementation)</t>
-  </si>
-  <si>
-    <t>Just adapted tutorial code to use strings,  borrower list is just set to NULL</t>
-  </si>
-  <si>
-    <t>bst_test - tests insertion to the left, insertion to the right, and large number of random insertions (see rand_string function for generating test strings); test deletion for zero, one and two child case, and deletion of the root.</t>
-  </si>
-  <si>
-    <t>Noticed that program crashed on destroy_bst.  Did not occur for an empty bst, so checked memory allocations and discovered error with malloc in insert_bst.
-Noticed an issue when book titles have spaces - decided to just remove spaces for now, may fix later.</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -132,6 +106,30 @@
   </si>
   <si>
     <t>https://github.com/BronsonKBilling/KIT205_575952</t>
+  </si>
+  <si>
+    <t>Not a milestone - Created all necessary functions and files for implentation of prototype 1, a linked list within a linked list.</t>
+  </si>
+  <si>
+    <t>Adapted tutorial code, mainly from the week 6 tutorial. Also used ChatGPT to learn about generic types (void*)</t>
+  </si>
+  <si>
+    <t>create_record
+compare_records
+print_records
+test_records
+create_list
+print_list
+print_one_to_many
+insert
+test_list</t>
+  </si>
+  <si>
+    <t>These functions have not been implemented. The only implemented function among those listed is create_list(), as this was easily adapted from the tutorial code. This commit is to give a structure and a plan for my future development of the first prototype. It aims to be the scaffolding for the prototype and prove that I have thought about how I wish to implement it before actually implementing it.</t>
+  </si>
+  <si>
+    <t>test_records - Tests all functions of the records file. Not yet implemented
+test_list - Tests all functions of the linked_list file. Not yet implemented</t>
   </si>
 </sst>
 </file>
@@ -242,14 +240,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -591,12 +589,30 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="4">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9CB2C690-049A-414B-9843-69F7EC8726FD}">
+  <we:reference id="8caa46f3-14c0-4824-9208-8faac4bf2c1e" version="1.0.0.7" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,43 +628,43 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+        <v>16</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="11">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10">
         <v>45760</v>
       </c>
     </row>
@@ -664,13 +680,13 @@
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>5</v>
@@ -678,7 +694,7 @@
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="81.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -690,30 +706,30 @@
         <v>4</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45766</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MILESTONE - Implementation of 'record.c' has been complete, along with testing function
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/bronson_billing_utas_edu_au/Documents/2025 - S1/KIT205/KIT205_575952/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{A0285DF0-F68A-42CE-9430-462A5BA0CC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFECC979-F2DE-46D5-83C0-BF56C61D0C76}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{A0285DF0-F68A-42CE-9430-462A5BA0CC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF6BC69-60AB-455A-9FD5-07F89AC203BF}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="19245" yWindow="3405" windowWidth="17355" windowHeight="14925" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>Not a milestone - Created all necessary functions and files for implentation of prototype 1, a linked list within a linked list.</t>
   </si>
   <si>
-    <t>Adapted tutorial code, mainly from the week 6 tutorial. Also used ChatGPT to learn about generic types (void*)</t>
-  </si>
-  <si>
     <t>create_record
 compare_records
 print_records
@@ -130,6 +127,9 @@
   <si>
     <t>test_records - Tests all functions of the records file. Not yet implemented
 test_list - Tests all functions of the linked_list file. Not yet implemented</t>
+  </si>
+  <si>
+    <t>Adapted tutorial code, mainly from the week 6 tutorial. Also used ChatGPT to learn about generic types (void*) and enums.</t>
   </si>
 </sst>
 </file>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,16 +720,16 @@
         <v>45766</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated devlog for previous commit
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/bronson_billing_utas_edu_au/Documents/2025 - S1/KIT205/KIT205_575952/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{A0285DF0-F68A-42CE-9430-462A5BA0CC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF6BC69-60AB-455A-9FD5-07F89AC203BF}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{A0285DF0-F68A-42CE-9430-462A5BA0CC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3062817-7765-4F27-83A6-68622A245458}"/>
   <bookViews>
     <workbookView xWindow="19245" yWindow="3405" windowWidth="17355" windowHeight="14925" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -47,37 +47,12 @@
     <t>GitHub Commit Dates</t>
   </si>
   <si>
-    <t>new_list
-insert_at_front
-print_list
-delete_from_list
-destroy_list</t>
-  </si>
-  <si>
-    <t>ChatGPT used to speed implementation of C string functions
-https://www.geeksforgeeks.org/c-program-to-implement-singly-linked-list/
-See code comments for further details</t>
-  </si>
-  <si>
     <t>Implementation/Testing Notes</t>
   </si>
   <si>
-    <t>Had issue where random characters were printed.  Used breakpoints and watches to identify that new_list was not correctly initialised.</t>
-  </si>
-  <si>
-    <t>29/07/2024
-1/08/2024</t>
-  </si>
-  <si>
-    <t>linked_list_test - tests insertion in empty and large linked lists; deletion from the front, middle, and rear</t>
-  </si>
-  <si>
     <t>Test Functions</t>
   </si>
   <si>
-    <t>Linked list implementation for strings to be used for book borrower list</t>
-  </si>
-  <si>
     <t>Functions implented/updated</t>
   </si>
   <si>
@@ -109,12 +84,30 @@
   </si>
   <si>
     <t>Not a milestone - Created all necessary functions and files for implentation of prototype 1, a linked list within a linked list.</t>
+  </si>
+  <si>
+    <t>These functions have not been implemented. The only implemented function among those listed is create_list(), as this was easily adapted from the tutorial code. This commit is to give a structure and a plan for my future development of the first prototype. It aims to be the scaffolding for the prototype and prove that I have thought about how I wish to implement it before actually implementing it.</t>
+  </si>
+  <si>
+    <t>Adapted tutorial code, mainly from the week 6 tutorial. Also used ChatGPT to learn about generic types (void*) and enums.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not a milestone - Implemented all functions in 'record.c' and implemented a testing function. </t>
   </si>
   <si>
     <t>create_record
 compare_records
 print_records
-test_records
+test_records</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to troubleshoot some errors. Also was used to gain a further understanding of enums, particularly why they cannot be set to NULL.</t>
+  </si>
+  <si>
+    <t>create_record
+compare_records
+print_records
+test_record
 create_list
 print_list
 print_one_to_many
@@ -122,14 +115,14 @@
 test_list</t>
   </si>
   <si>
-    <t>These functions have not been implemented. The only implemented function among those listed is create_list(), as this was easily adapted from the tutorial code. This commit is to give a structure and a plan for my future development of the first prototype. It aims to be the scaffolding for the prototype and prove that I have thought about how I wish to implement it before actually implementing it.</t>
-  </si>
-  <si>
-    <t>test_records - Tests all functions of the records file. Not yet implemented
+    <t>test_record- Tests all functions of the records file. Not yet implemented
 test_list - Tests all functions of the linked_list file. Not yet implemented</t>
   </si>
   <si>
-    <t>Adapted tutorial code, mainly from the week 6 tutorial. Also used ChatGPT to learn about generic types (void*) and enums.</t>
+    <t>test_record - Tests all functions in 'record.c' file. Tests that error checks within these functions work as intended and that all execution paths are valid and work properly</t>
+  </si>
+  <si>
+    <t>Had an issue where enums could not be null. I needed to change the implementation of how enums are used in records by creating an 'unset' option.</t>
   </si>
 </sst>
 </file>
@@ -611,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,41 +621,41 @@
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B5" s="10">
         <v>45760</v>
@@ -680,56 +673,56 @@
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="81.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45766</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3">
         <v>45766</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated devlog for last commit
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B575E88-A1C4-48EB-89F9-AE0EB68FFD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DC2145-2764-4127-BAF8-27B7884979A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="3405" windowWidth="28245" windowHeight="14610" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="1530" yWindow="3810" windowWidth="17355" windowHeight="14925" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -143,6 +143,27 @@
   </si>
   <si>
     <t>Had an issue where enums could not be null. I needed to change the implementation of how enums are used in records by creating an 'unset' option. This commit shows up in the Github history as being made on the 20th of April, but it was originally made on the 19th. The commit message did not include 'MILESTONE' and needed to be reworded, this resulted in the date being changed.</t>
+  </si>
+  <si>
+    <t>Not a milestone - Implemented new functions in Record.c and fixed existing functions</t>
+  </si>
+  <si>
+    <t>compare_records
+print_records
+clone_record
+destroy_record
+change_int_identifier
+change_string_identifier
+test_record</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to troubleshoot errors and gain a better understanding of memory management and how pointers work. Was also used to gain an understanding of how I could test destroy_record. It helped me come to the conclusion that the funciton had been tested enough and that no further testing could be done</t>
+  </si>
+  <si>
+    <t>test_record - Now tests the new functions. Existing tests have been modified to incorporate the new functions</t>
+  </si>
+  <si>
+    <t>This change was necessary to ensure memory safety and scalability with the database. This commit especially aided my understanding of C and how memory works within C, and on a hardware level in general. I feel far more confident using C after this commit. This file will need to be expanded further in the future once the AVL tree is implemented, in order to incorporate the ability for Records to store lists and trees within their data field.</t>
   </si>
 </sst>
 </file>
@@ -204,7 +225,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -230,15 +251,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -247,7 +259,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -262,7 +274,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -275,16 +286,20 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -643,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,23 +676,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -687,18 +702,18 @@
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>45760</v>
       </c>
     </row>
@@ -706,95 +721,107 @@
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="81.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:7" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="15">
+        <v>45769</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C10" s="13">
         <v>45767</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G10" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C11" s="3">
         <v>45766</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
@@ -1093,12 +1120,20 @@
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Milestone - prototype 1 datastructures have been implemented and tested.
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DC2145-2764-4127-BAF8-27B7884979A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C0F77D-6E79-443E-946B-5C37B6E1A6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="3810" windowWidth="17355" windowHeight="14925" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -164,6 +164,33 @@
   </si>
   <si>
     <t>This change was necessary to ensure memory safety and scalability with the database. This commit especially aided my understanding of C and how memory works within C, and on a hardware level in general. I feel far more confident using C after this commit. This file will need to be expanded further in the future once the AVL tree is implemented, in order to incorporate the ability for Records to store lists and trees within their data field.</t>
+  </si>
+  <si>
+    <t>Milestone - Implemented all functions linked_list.c and implemented a testing function. All tests passed and this compiled successfully. This means that all prototype 1 data structures have been created</t>
+  </si>
+  <si>
+    <t>22/04/2025
+20/04/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create_node
+insert_at_front
+insert_at_rear
+insert_at_middle_from_front
+insert_at_middle_from_rear
+insert
+delete_node
+test_list
+</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to again learn more about memory and pointers. It was used to a far lesser extent than in previous commits. The tutorial code was also used as both a reference for the code and was partially directly used.</t>
+  </si>
+  <si>
+    <t>test_list - Tests all functions in linked_list.c that need testing (notes about this are present in the function). The tests go through all possible execution paths and ensure that the functions work as intended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some functions need to make assumptions and these are noted in the comment headers of the functions. These assumptions reflect things that take place upstream of the function, normally things that have been planned for the database implementation. </t>
   </si>
 </sst>
 </file>
@@ -259,7 +286,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -300,6 +327,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -658,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,95 +771,108 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C10" s="15">
         <v>45769</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G10" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C11" s="13">
         <v>45767</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C11" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C12" s="3">
         <v>45766</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
@@ -1128,12 +1171,20 @@
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Implemented all functions aside from test_avl in avl_tree.c, updated devlog
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C0F77D-6E79-443E-946B-5C37B6E1A6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670D4C0C-06F1-477E-8FAB-747EB21C8CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -191,6 +191,33 @@
   </si>
   <si>
     <t xml:space="preserve">Some functions need to make assumptions and these are noted in the comment headers of the functions. These assumptions reflect things that take place upstream of the function, normally things that have been planned for the database implementation. </t>
+  </si>
+  <si>
+    <t>Not a milestone - Implemented all functions aside from test_avl in avl_tree.c. Also created a header file for it.</t>
+  </si>
+  <si>
+    <t>test_avl - not fully implemented. Only holdds adhoc tests</t>
+  </si>
+  <si>
+    <t>The tutorials, specifically the week 5 tutorial on BSTs, were used heavily. Code was copied from it, and functions were derivative of it. ChatGPT was used for gaining a slightly better understanding of how balancing the tree could be implemented but for the most part the balancing and insertion methods were derived from my notes on the weekly content.</t>
+  </si>
+  <si>
+    <t>create_avl
+find_avl_node
+find_avl
+find_left_right_height
+get_avl_node_height
+left_rotate
+right_rotate
+balance_tree
+insert_avl_node
+insert_avl
+print_avl_node
+print_avl
+test_avl</t>
+  </si>
+  <si>
+    <t>test_avl has been implemented with some adhoc tests that served purely to see the basic functionality of the functions. These are by no means exhaustive and do not at all match the format seen in other testing functions. This file also has more code from the tutorials than any other file. Both the linked list and record files were largely implemented with very little tutorial code and were largely custom. This file also uses a similar format of having wrapper functions and a wrapper struct as the BST file did in the week 5 tutorial.</t>
   </si>
 </sst>
 </file>
@@ -286,7 +313,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -316,9 +343,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -329,8 +353,8 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -688,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,11 +749,11 @@
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -752,135 +776,148 @@
       <c r="B6" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+    <row r="9" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
       <c r="B9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+    <row r="11" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C11" s="14">
         <v>45769</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11" s="10" t="s">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C12" s="12">
         <v>45767</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C13" s="3">
         <v>45766</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
@@ -1179,12 +1216,20 @@
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Milestone - Completed prototype 2 data structure (AVL tree). All funcitons have been implemented and thoroughly tested along all execution paths
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670D4C0C-06F1-477E-8FAB-747EB21C8CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBEC8B0-BFDA-4E2A-830C-1AE21962339A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -218,6 +218,25 @@
   </si>
   <si>
     <t>test_avl has been implemented with some adhoc tests that served purely to see the basic functionality of the functions. These are by no means exhaustive and do not at all match the format seen in other testing functions. This file also has more code from the tutorials than any other file. Both the linked list and record files were largely implemented with very little tutorial code and were largely custom. This file also uses a similar format of having wrapper functions and a wrapper struct as the BST file did in the week 5 tutorial.</t>
+  </si>
+  <si>
+    <t>Milestone - Fully implemented all function in avl_tree.c by testing them thoroughly along all possible execution paths. This means that prototype 2 data structures are now implemented.</t>
+  </si>
+  <si>
+    <t>get_avl_node_height
+insert_avl_node
+delete_avl
+delete_avl_children
+test_avl</t>
+  </si>
+  <si>
+    <t>ChatGPT was used sparingly for some basic bug finding. As this assignment grows my knowledge of both C and Visual Studio testing tools, I am relying less and less on resources for fixing my code. I find it easier now to fix it myself and often find ChatGPT's suggestions to be a hinderance and incorrect. The tutorials also were used and tests written for the week 5 tutorial on BSTs were retrofitted for testing AVLs.</t>
+  </si>
+  <si>
+    <t>test_avl - Fully implemented. Now tests all execution paths and possible scenarios. There are many notes justifying certain decisions within this test function.</t>
+  </si>
+  <si>
+    <t>Now that this file has been fully implemented. The record and linked_list files can be expanded to incorporate this file.</t>
   </si>
 </sst>
 </file>
@@ -313,7 +332,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -355,6 +374,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -712,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="E5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,137 +817,150 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
       <c r="B9" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C9" s="12">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+    <row r="12" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C12" s="14">
         <v>45769</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12" s="10" t="s">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C13" s="12">
         <v>45767</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C14" s="3">
         <v>45766</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
@@ -1224,12 +1259,20 @@
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Implemented functions for database.c. Also makde changes to avl_tree and linked_list
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBEC8B0-BFDA-4E2A-830C-1AE21962339A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02530CC5-CA40-490A-969C-E77ED6656837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -237,6 +237,34 @@
   </si>
   <si>
     <t>Now that this file has been fully implemented. The record and linked_list files can be expanded to incorporate this file.</t>
+  </si>
+  <si>
+    <t>Not a milestone - Implemented functions for database.c. Also made changes to avl_tree to accommodate the database better. linked_list had a function name refactored as well for clarity</t>
+  </si>
+  <si>
+    <t>insert_list
+print_avl_node_without_tree
+print_avl_without_tree
+print_events
+print_fighters_in_event
+add_fighter_list
+add_fighter_avl
+add_fighter_to_event
+add_event
+print_events)of_fighter_list
+print_events_of_fighter_avl
+print_events_of_fighter
+test_database</t>
+  </si>
+  <si>
+    <t>No other resources were used for this commit.</t>
+  </si>
+  <si>
+    <t>test_database - This currently only includes unstructured adhoc tests that aimed to prove that the functions work in their most basic use cases. Functions in database.c require further testing</t>
+  </si>
+  <si>
+    <t>It has become obvious across multiple files that the commenting style is somewhat inconsistent. There is (I feel) a good amount of comments written, but the style of them and the display needs to be made uniform. There are also some functions that have far less commenting than others. A commit will need to focus solely on updating comments.
+It has also come to my attention that my use of a doubly linked list may have been somewhat unnecessary. It was meant to cut down the time it takes to search for records. But later on I realised that it would be pointless when searching for fighters, as the alphabetical order of names can be quite random. I found that it would only be useful for searching from the tail or head of the list that contains event codes, as if the tail was an event such as 315, and the user was searching for event 310, then it can be easily calculated that it would be better to go from the tail. However the most time complex function of the database, which is finding which events a fighter has fought in, requires every event to be searched. This means that the usefulness of the doubly linked list is lessened.</t>
   </si>
 </sst>
 </file>
@@ -332,7 +360,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -374,9 +402,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -734,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,158 +842,170 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+    <row r="9" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C9" s="12">
-        <v>45772</v>
+        <v>45774</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C10" s="12">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+    <row r="13" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C13" s="14">
         <v>45769</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13" s="10" t="s">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C14" s="12">
         <v>45767</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C15" s="3">
         <v>45766</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
@@ -1267,12 +1304,20 @@
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Milestone - database.c has been fully implemented now that test_database() is complete. All database functions have been tested.
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02530CC5-CA40-490A-969C-E77ED6656837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51CE3A3-566A-4F53-B63E-B186951F6DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19590" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -265,6 +265,24 @@
   <si>
     <t>It has become obvious across multiple files that the commenting style is somewhat inconsistent. There is (I feel) a good amount of comments written, but the style of them and the display needs to be made uniform. There are also some functions that have far less commenting than others. A commit will need to focus solely on updating comments.
 It has also come to my attention that my use of a doubly linked list may have been somewhat unnecessary. It was meant to cut down the time it takes to search for records. But later on I realised that it would be pointless when searching for fighters, as the alphabetical order of names can be quite random. I found that it would only be useful for searching from the tail or head of the list that contains event codes, as if the tail was an event such as 315, and the user was searching for event 310, then it can be easily calculated that it would be better to go from the tail. However the most time complex function of the database, which is finding which events a fighter has fought in, requires every event to be searched. This means that the usefulness of the doubly linked list is lessened.</t>
+  </si>
+  <si>
+    <t>Milestone - Fully implemented all functions in database.c by testing them thorougly along all execution paths. The database has now been fully implemented and both the many to many and one to many relationships can be printed successfully. Some funcitons in database.c have also been modified, mainly to make them more user friendly by giving helpful messages.</t>
+  </si>
+  <si>
+    <t>test_database
+print_events_of_fighter_avl
+print_events_of_fighter_list
+print_events_of_fighter
+add_fighter_avl
+add_fighter_list
+add_fighter_to_event</t>
+  </si>
+  <si>
+    <t>test_database - This function is now fully implemented and tests all functions in database.c along all possible execution paths.</t>
+  </si>
+  <si>
+    <t>While the assignment spec does not say to have the database be made to accommodate users, the theme of the entire project for me has been to accommodate a potential upgrade of the program to accommodate user input and usage. This is why the database will give helpful error messages and will say what it is printing prior to printing it. This decision also informed my data structure choices.</t>
   </si>
 </sst>
 </file>
@@ -360,7 +378,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -402,6 +420,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -759,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,180 +863,193 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45776</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="12">
         <v>45774</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="12">
-        <v>45772</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C11" s="12">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+    <row r="14" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C14" s="14">
         <v>45769</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F14" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G14" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14" s="10" t="s">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C15" s="12">
         <v>45767</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+    <row r="16" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C16" s="3">
         <v>45766</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1023,7 +1057,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1031,7 +1065,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1039,7 +1073,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1047,7 +1081,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1055,7 +1089,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1063,7 +1097,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1071,7 +1105,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1079,7 +1113,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1087,7 +1121,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1095,7 +1129,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1103,7 +1137,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1111,7 +1145,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1119,7 +1153,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1127,7 +1161,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1312,12 +1346,20 @@
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
data_creator.py was added to make data acceptable for use. More details on data collection in devlog
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51CE3A3-566A-4F53-B63E-B186951F6DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494C039B-78AF-4ED1-9733-BACBE6204628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19590" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="36645" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -283,6 +283,22 @@
   </si>
   <si>
     <t>While the assignment spec does not say to have the database be made to accommodate users, the theme of the entire project for me has been to accommodate a potential upgrade of the program to accommodate user input and usage. This is why the database will give helpful error messages and will say what it is printing prior to printing it. This decision also informed my data structure choices.</t>
+  </si>
+  <si>
+    <t>Not a milestone - Added a python file that was used to turn data from dataset into a format that can be used for testing the database functions and data structures.</t>
+  </si>
+  <si>
+    <t>main() (data_creator.py)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to help create the regular expression that matches if a record has the format 'UFC [event code]'
+Kaggle was used to retrieve a dataset of all UFC events from 1996-2024. This is the dataset that is modified to create the testing dataset. The link for this dataset is: https://www.kaggle.com/datasets/maksbasher/ufc-complete-dataset-all-events-1996-2024?resource=download</t>
+  </si>
+  <si>
+    <t>Dataset was taken from Kaggle (more information in resources used section) and converted into testing data using Python script. The output of the Python script is now in the file 'data.txt' while the original dataset is in the file 'medium_dataset.csv'.</t>
   </si>
 </sst>
 </file>
@@ -378,7 +394,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -420,6 +436,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -780,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,199 +882,212 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="12">
+        <v>45776</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <v>45776</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C11" s="12">
         <v>45774</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="12">
-        <v>45772</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C12" s="12">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+    <row r="15" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C15" s="14">
         <v>45769</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G15" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15" s="10" t="s">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C16" s="12">
         <v>45767</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+    <row r="17" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>45766</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -1354,12 +1386,20 @@
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Data was re-generated to allow for larger M and N values. Data used prior for testing was far too small to conduct any meaningful tests
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494C039B-78AF-4ED1-9733-BACBE6204628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56684502-6371-4C43-BF2E-EDCD35FE3AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36645" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
+    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t>Dataset was taken from Kaggle (more information in resources used section) and converted into testing data using Python script. The output of the Python script is now in the file 'data.txt' while the original dataset is in the file 'medium_dataset.csv'.</t>
+  </si>
+  <si>
+    <t>Not  a milestone - Regenerated data for testing. Prior dataset was not large enough for any meaningful tests as the M and N values were just too small.</t>
+  </si>
+  <si>
+    <t>generate_ufc_dataset_to_file()</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to write the entirety of the python data generation file</t>
+  </si>
+  <si>
+    <t>ChatGPT created all code to generate the dataset. Previous data is still held in the repo as an artifact and can still be used for testing, it is just not suitable for doing any meaningful tests of the prototypes.</t>
   </si>
 </sst>
 </file>
@@ -434,14 +446,14 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -799,9 +811,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -836,11 +848,11 @@
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -882,220 +894,233 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
       <c r="B9" s="10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C9" s="12">
-        <v>45776</v>
+        <v>45777</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="12">
+        <v>45776</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>45776</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+    <row r="12" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C12" s="12">
         <v>45774</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="12">
-        <v>45772</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C13" s="12">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G15" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+    <row r="16" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C16" s="14">
         <v>45769</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G16" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16" s="10" t="s">
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C17" s="12">
         <v>45767</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C17" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C18" s="3">
         <v>45766</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -1394,12 +1419,20 @@
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Milestone - Completed prototype evaluation testing function. All necessary code and tests have now been written and are executed in the main() function.
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56684502-6371-4C43-BF2E-EDCD35FE3AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2752F66-F51B-4E69-9D30-0CFC33EA8986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -311,6 +311,23 @@
   </si>
   <si>
     <t>ChatGPT created all code to generate the dataset. Previous data is still held in the repo as an artifact and can still be used for testing, it is just not suitable for doing any meaningful tests of the prototypes.</t>
+  </si>
+  <si>
+    <t>Milestone - Evaluation of prototypes has been completed and the function to evaluate prototypes is now called in main alongside all other unit tests. This means that all necessary code for the assignment has been written</t>
+  </si>
+  <si>
+    <t>read_data
+time_many_to_many
+evaluate_database</t>
+  </si>
+  <si>
+    <t>ChatGPT was used to write some of the read_data function, the lines written by ChatGPT are clearly marked in the function. The week 9 tutorial was used to learn about file reading and the week 4 tutorial code for timing code execution was used to time the many to many prototype function</t>
+  </si>
+  <si>
+    <t>evaluate_database - Does not necessarily test the other functions implemented in this commit, but tests the prototypes and how they handle different m and n values.</t>
+  </si>
+  <si>
+    <t>The read_data function is taking a very long time to read all  2.5M records. This is to be expected, but a warning is still included in the evaluate_database function. The read_data function was modified many times to execute in the least amount of time possible.</t>
   </si>
 </sst>
 </file>
@@ -811,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,241 +911,254 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C9" s="12">
         <v>45777</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="12">
+        <v>45777</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="12">
-        <v>45776</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G10" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="12">
+        <v>45776</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <v>45776</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+    <row r="13" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C13" s="12">
         <v>45774</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="12">
-        <v>45772</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C14" s="12">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+    <row r="17" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C17" s="14">
         <v>45769</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E17" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G17" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17" s="10" t="s">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C18" s="12">
         <v>45767</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+    <row r="19" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C18" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C19" s="3">
         <v>45766</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
@@ -1427,12 +1457,20 @@
       <c r="G57" s="2"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated comments for readability, reconfigured where new lines are placed in testing files and added header print to each
</commit_message>
<xml_diff>
--- a/DevLog.xlsx
+++ b/DevLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bronson\OneDrive - University of Tasmania\2025 - S1\KIT205\KIT205_575952\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2752F66-F51B-4E69-9D30-0CFC33EA8986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3D086E-1435-417D-8172-072FD566E261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{E01BF87A-8E79-4CC1-91E6-E14A4898A4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Milestone Description</t>
   </si>
@@ -328,6 +328,18 @@
   </si>
   <si>
     <t>The read_data function is taking a very long time to read all  2.5M records. This is to be expected, but a warning is still included in the evaluate_database function. The read_data function was modified many times to execute in the least amount of time possible.</t>
+  </si>
+  <si>
+    <t>Not a milestone - cleaned up code files and improved commenting</t>
+  </si>
+  <si>
+    <t>No logic was updated, only comments. The majority of functions were updated</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>This was needed to ensure the maintainability and readability of the code.</t>
   </si>
 </sst>
 </file>
@@ -828,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4D48D-C417-45FE-8518-4215B0DD66E3}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,262 +923,275 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="10" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C9" s="12">
         <v>45777</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C10" s="12">
         <v>45777</v>
       </c>
       <c r="D10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="12">
+        <v>45777</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="12">
-        <v>45776</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="12">
+        <v>45776</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>45776</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+    <row r="14" spans="1:7" ht="246.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C14" s="12">
         <v>45774</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="12">
-        <v>45772</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C15" s="12">
-        <v>45771</v>
+        <v>45772</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="12">
+        <v>45771</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="18" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C18" s="14">
         <v>45769</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G18" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18" s="10" t="s">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C19" s="12">
         <v>45767</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G19" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+    <row r="20" spans="1:7" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C19" s="3">
-        <v>45766</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C20" s="3">
         <v>45766</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45766</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
@@ -1465,12 +1490,20 @@
       <c r="G58" s="2"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>